<commit_message>
[23.12.21 18:46] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6544801-A141-4916-B25D-9DB3E071927D}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB295EF5-3F4B-4624-92C5-41E6C123978E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="MISSION.TYPE" sheetId="3" r:id="rId1"/>
@@ -1570,7 +1570,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1670,7 +1670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1692,6 +1692,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -2103,7 +2107,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2401,11 +2405,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
@@ -2414,7 +2418,7 @@
     <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2427,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2432,7 +2436,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2441,7 +2445,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2450,7 +2454,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2459,14 +2463,14 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2475,14 +2479,14 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -2514,7 +2518,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -2529,7 +2533,7 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -2544,7 +2548,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -2559,7 +2563,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
@@ -2574,7 +2578,7 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>32</v>
       </c>
@@ -2589,7 +2593,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -2604,7 +2608,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
@@ -2619,7 +2623,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
@@ -2634,7 +2638,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -2649,7 +2653,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
@@ -2664,7 +2668,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>50</v>
       </c>
@@ -2679,7 +2683,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>53</v>
       </c>
@@ -2694,7 +2698,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>56</v>
       </c>
@@ -2709,7 +2713,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -2724,7 +2728,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>62</v>
       </c>
@@ -2739,7 +2743,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>65</v>
       </c>
@@ -2754,7 +2758,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>68</v>
       </c>
@@ -2769,7 +2773,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>71</v>
       </c>
@@ -2784,7 +2788,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>74</v>
       </c>
@@ -2799,7 +2803,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>77</v>
       </c>
@@ -2814,7 +2818,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>80</v>
       </c>
@@ -2829,7 +2833,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>83</v>
       </c>
@@ -2844,7 +2848,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>86</v>
       </c>
@@ -2859,7 +2863,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>89</v>
       </c>
@@ -2874,7 +2878,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>92</v>
       </c>
@@ -2889,14 +2893,14 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="13" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -2904,14 +2908,14 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -2919,7 +2923,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>101</v>
       </c>
@@ -2934,7 +2938,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>104</v>
       </c>
@@ -2949,7 +2953,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>107</v>
       </c>
@@ -2964,7 +2968,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>110</v>
       </c>
@@ -2979,7 +2983,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>113</v>
       </c>
@@ -2994,7 +2998,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>116</v>
       </c>
@@ -3009,7 +3013,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>119</v>
       </c>
@@ -3024,7 +3028,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>122</v>
       </c>
@@ -3039,7 +3043,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>125</v>
       </c>
@@ -3054,7 +3058,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>128</v>
       </c>
@@ -3069,7 +3073,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>131</v>
       </c>
@@ -3084,7 +3088,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>134</v>
       </c>
@@ -3099,7 +3103,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>137</v>
       </c>
@@ -3114,7 +3118,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>140</v>
       </c>
@@ -3129,7 +3133,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>143</v>
       </c>
@@ -3144,7 +3148,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>146</v>
       </c>
@@ -3159,7 +3163,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>149</v>
       </c>
@@ -3174,7 +3178,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>152</v>
       </c>
@@ -3189,7 +3193,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>155</v>
       </c>
@@ -3204,7 +3208,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>158</v>
       </c>
@@ -3219,7 +3223,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>161</v>
       </c>
@@ -3234,7 +3238,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>164</v>
       </c>
@@ -3249,7 +3253,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>167</v>
       </c>
@@ -3264,7 +3268,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>170</v>
       </c>
@@ -3279,7 +3283,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>173</v>
       </c>
@@ -3294,7 +3298,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>176</v>
       </c>
@@ -3309,7 +3313,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>179</v>
       </c>
@@ -3324,7 +3328,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>182</v>
       </c>
@@ -3339,7 +3343,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>185</v>
       </c>
@@ -3354,7 +3358,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>188</v>
       </c>
@@ -3369,7 +3373,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>191</v>
       </c>
@@ -3384,7 +3388,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>194</v>
       </c>
@@ -3399,7 +3403,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>197</v>
       </c>
@@ -3414,7 +3418,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>200</v>
       </c>
@@ -3429,7 +3433,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>203</v>
       </c>
@@ -3444,7 +3448,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>206</v>
       </c>
@@ -3459,7 +3463,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>209</v>
       </c>
@@ -3474,7 +3478,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>212</v>
       </c>
@@ -3489,7 +3493,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>215</v>
       </c>
@@ -3504,7 +3508,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>218</v>
       </c>
@@ -3519,7 +3523,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>221</v>
       </c>
@@ -3534,7 +3538,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>224</v>
       </c>
@@ -3549,7 +3553,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>227</v>
       </c>
@@ -3564,7 +3568,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>230</v>
       </c>
@@ -3579,7 +3583,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>233</v>
       </c>
@@ -3594,7 +3598,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>236</v>
       </c>
@@ -3609,7 +3613,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>239</v>
       </c>
@@ -3624,7 +3628,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>242</v>
       </c>
@@ -3639,7 +3643,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>245</v>
       </c>
@@ -3654,7 +3658,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>248</v>
       </c>
@@ -3669,7 +3673,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>251</v>
       </c>
@@ -3684,7 +3688,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>254</v>
       </c>
@@ -3699,7 +3703,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>257</v>
       </c>
@@ -3714,7 +3718,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>260</v>
       </c>
@@ -3729,7 +3733,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>263</v>
       </c>
@@ -3744,7 +3748,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>265</v>
       </c>
@@ -3759,7 +3763,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>268</v>
       </c>
@@ -3774,7 +3778,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>271</v>
       </c>
@@ -3789,7 +3793,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>274</v>
       </c>
@@ -3804,7 +3808,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>277</v>
       </c>
@@ -3819,7 +3823,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>280</v>
       </c>
@@ -3834,7 +3838,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>283</v>
       </c>
@@ -3849,7 +3853,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>286</v>
       </c>
@@ -3864,7 +3868,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>289</v>
       </c>
@@ -3879,7 +3883,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>292</v>
       </c>
@@ -3894,7 +3898,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>295</v>
       </c>
@@ -3909,7 +3913,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>298</v>
       </c>
@@ -3924,7 +3928,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>301</v>
       </c>
@@ -3939,7 +3943,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>304</v>
       </c>
@@ -3954,7 +3958,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>307</v>
       </c>
@@ -3967,7 +3971,7 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>309</v>
       </c>
@@ -3980,7 +3984,7 @@
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>311</v>
       </c>
@@ -3995,7 +3999,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>314</v>
       </c>
@@ -4010,7 +4014,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>317</v>
       </c>
@@ -4025,7 +4029,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>320</v>
       </c>
@@ -4040,7 +4044,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>323</v>
       </c>
@@ -4055,7 +4059,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>325</v>
       </c>
@@ -4070,7 +4074,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>328</v>
       </c>
@@ -4085,7 +4089,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>331</v>
       </c>
@@ -4100,7 +4104,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>334</v>
       </c>
@@ -4115,7 +4119,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>337</v>
       </c>
@@ -4130,7 +4134,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>340</v>
       </c>
@@ -4145,7 +4149,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>343</v>
       </c>
@@ -4160,7 +4164,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>346</v>
       </c>
@@ -4175,7 +4179,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>349</v>
       </c>
@@ -4190,7 +4194,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>352</v>
       </c>
@@ -4205,7 +4209,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>355</v>
       </c>
@@ -4220,7 +4224,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>358</v>
       </c>
@@ -4235,7 +4239,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>361</v>
       </c>
@@ -4250,7 +4254,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>364</v>
       </c>
@@ -4265,7 +4269,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>367</v>
       </c>
@@ -4280,7 +4284,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>370</v>
       </c>
@@ -4295,7 +4299,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>373</v>
       </c>
@@ -4310,7 +4314,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>376</v>
       </c>
@@ -4325,7 +4329,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>379</v>
       </c>
@@ -4340,7 +4344,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>382</v>
       </c>
@@ -4355,7 +4359,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>385</v>
       </c>
@@ -4370,7 +4374,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>388</v>
       </c>
@@ -4385,7 +4389,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>391</v>
       </c>
@@ -4400,7 +4404,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>394</v>
       </c>
@@ -4415,7 +4419,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>397</v>
       </c>
@@ -4430,7 +4434,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>400</v>
       </c>
@@ -4445,7 +4449,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>403</v>
       </c>
@@ -4460,7 +4464,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>406</v>
       </c>
@@ -4475,7 +4479,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>409</v>
       </c>
@@ -4490,7 +4494,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>412</v>
       </c>
@@ -4505,7 +4509,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>415</v>
       </c>
@@ -4520,7 +4524,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>418</v>
       </c>
@@ -4535,7 +4539,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>421</v>
       </c>
@@ -4550,7 +4554,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>424</v>
       </c>
@@ -4565,7 +4569,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>427</v>
       </c>
@@ -4580,7 +4584,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>430</v>
       </c>
@@ -4595,7 +4599,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>433</v>
       </c>
@@ -4610,7 +4614,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>436</v>
       </c>
@@ -4625,7 +4629,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>439</v>
       </c>
@@ -4640,7 +4644,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>442</v>
       </c>
@@ -4655,7 +4659,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>445</v>
       </c>
@@ -4670,7 +4674,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>448</v>
       </c>
@@ -4685,7 +4689,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>451</v>
       </c>
@@ -4700,7 +4704,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>454</v>
       </c>
@@ -4713,7 +4717,7 @@
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>456</v>
       </c>
@@ -4728,7 +4732,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>459</v>
       </c>
@@ -4743,7 +4747,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>462</v>
       </c>
@@ -4758,7 +4762,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>465</v>
       </c>
@@ -4773,7 +4777,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>468</v>
       </c>
@@ -4788,7 +4792,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>471</v>
       </c>
@@ -4803,7 +4807,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>474</v>
       </c>
@@ -4818,7 +4822,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>477</v>
       </c>
@@ -4833,7 +4837,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>480</v>
       </c>
@@ -4848,7 +4852,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>483</v>
       </c>
@@ -4863,7 +4867,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>486</v>
       </c>
@@ -4878,7 +4882,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>489</v>
       </c>
@@ -4893,7 +4897,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>491</v>
       </c>
@@ -4908,7 +4912,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>493</v>
       </c>
@@ -4940,7 +4944,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -4948,7 +4952,7 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4956,7 +4960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4964,7 +4968,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4972,7 +4976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4980,7 +4984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4988,13 +4992,13 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -5002,13 +5006,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -5022,7 +5026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>497</v>
       </c>
@@ -5034,7 +5038,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>499</v>
       </c>
@@ -5046,7 +5050,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>501</v>
       </c>
@@ -5058,7 +5062,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>503</v>
       </c>
@@ -5070,7 +5074,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>505</v>
       </c>
@@ -5082,7 +5086,7 @@
       </c>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>507</v>
       </c>
@@ -5103,15 +5107,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5f25723db95d46bd813c254178c12b28">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc30f4eda6069462a66ebc021061e28" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5519,6 +5514,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5572,13 +5576,47 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7AA67-47B2-4825-997F-EB2CD9778FFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7AA67-47B2-4825-997F-EB2CD9778FFB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.01.09 17:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB295EF5-3F4B-4624-92C5-41E6C123978E}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A1811-3E3C-48B8-AE4B-6661EDE24DE0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="MISSION.TYPE" sheetId="3" r:id="rId1"/>
@@ -1622,7 +1622,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1638,6 +1638,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,7 +1676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1696,6 +1702,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -2405,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,16 +3309,16 @@
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="15" t="s">
         <v>178</v>
       </c>
       <c r="E63" s="7"/>
@@ -3359,16 +3369,16 @@
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="15" t="s">
         <v>190</v>
       </c>
       <c r="E67" s="7"/>
@@ -5515,15 +5525,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -5575,6 +5576,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7AA67-47B2-4825-997F-EB2CD9778FFB}">
   <ds:schemaRefs>
@@ -5596,27 +5606,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.01.10 11:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="408" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A1811-3E3C-48B8-AE4B-6661EDE24DE0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
+    <workbookView minimized="1" xWindow="705" yWindow="4290" windowWidth="21600" windowHeight="11295" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="MISSION.TYPE" sheetId="3" r:id="rId1"/>
@@ -2415,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5117,8 +5117,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5f25723db95d46bd813c254178c12b28">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc30f4eda6069462a66ebc021061e28" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -5163,6 +5163,7 @@
                 <xsd:element ref="ns2:Ticket_x0020_Changement" minOccurs="0"/>
                 <xsd:element ref="ns2:Environnement" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5424,6 +5425,11 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="54" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -5586,23 +5592,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBA7AA67-47B2-4825-997F-EB2CD9778FFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FED4B9AA-8877-43C0-9BF1-4CF4C039AF65}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.02.16 09:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="438" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95659836-F308-4891-B7DE-801154F413D1}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A637A2A3-42A6-44C4-AB01-FBD8EFEF4B4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
@@ -126,114 +126,6 @@
     <t>Une ellipse définie par 3 points : la position des 2 foyers et une position sur le contour.</t>
   </si>
   <si>
-    <t>/SAV/ASC</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_DIFFICULTACCSS</t>
-  </si>
-  <si>
-    <t>/GEN/RECVRY</t>
-  </si>
-  <si>
-    <t>/RSC/SAR/FR_VLN</t>
-  </si>
-  <si>
-    <t>/SAV/ASC/FR_PPL/LIFT</t>
-  </si>
-  <si>
-    <t>/SAV/RHD</t>
-  </si>
-  <si>
-    <t>/SAV/RTA</t>
-  </si>
-  <si>
-    <t>/SAV/SARCSL</t>
-  </si>
-  <si>
-    <t>/FFST/FR_FIRE</t>
-  </si>
-  <si>
-    <t>/FSTT/RRHAZ/FR_CO</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_ANI/DGR</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_ANI/INJ</t>
-  </si>
-  <si>
-    <t>/INT/RECCE/FR_CBRNHZ</t>
-  </si>
-  <si>
-    <t>/INT/RECCE/FR_DIS/LNDSLD</t>
-  </si>
-  <si>
-    <t>/INT/RECCE/FR_DIS/SDCLPS</t>
-  </si>
-  <si>
-    <t>/INT/RECCE/FR_FLD</t>
-  </si>
-  <si>
-    <t>/INT/RECCE/FR_SMLL</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_DRG/MIND</t>
-  </si>
-  <si>
-    <t>/FR_MED/REGLTN</t>
-  </si>
-  <si>
-    <t>/GEN/SUPRTN</t>
-  </si>
-  <si>
-    <t>/REC/PRVCNP</t>
-  </si>
-  <si>
-    <t>/RSC/MEDEVC</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_CNT</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_MED</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_PARAMD</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_PPL/GRP</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_PSYPHY</t>
-  </si>
-  <si>
-    <t>/INT/RECCE</t>
-  </si>
-  <si>
-    <t>/SAV</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_TRNSP/AMB</t>
-  </si>
-  <si>
-    <t>/GEN/TRNSP</t>
-  </si>
-  <si>
-    <t>/GEN/TRNSP/FR_SECNDRY</t>
-  </si>
-  <si>
-    <t>/GEN/TRNSPN</t>
-  </si>
-  <si>
-    <t>/OPR/LOG</t>
-  </si>
-  <si>
-    <t>/SAV/AR/FR_PPL/OBS</t>
-  </si>
-  <si>
-    <t>/FSTT/TA/FR_CLRACCSS</t>
-  </si>
-  <si>
     <t>Besoin secouriste / personne(s) blesse(es)</t>
   </si>
   <si>
@@ -418,6 +310,114 @@
   </si>
   <si>
     <t>20240112_Effets à obtenir_Mission_Type</t>
+  </si>
+  <si>
+    <t>SAV/ASC</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_DIFFICULTACCSS</t>
+  </si>
+  <si>
+    <t>GEN/RECVRY</t>
+  </si>
+  <si>
+    <t>RSC/SAR/FR_VLN</t>
+  </si>
+  <si>
+    <t>SAV/ASC/FR_PPL/LIFT</t>
+  </si>
+  <si>
+    <t>SAV/RHD</t>
+  </si>
+  <si>
+    <t>SAV/RTA</t>
+  </si>
+  <si>
+    <t>SAV/SARCSL</t>
+  </si>
+  <si>
+    <t>FFST/FR_FIRE</t>
+  </si>
+  <si>
+    <t>FSTT/RRHAZ/FR_CO</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_ANI/DGR</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_ANI/INJ</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_CBRNHZ</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_DIS/LNDSLD</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_DIS/SDCLPS</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_FLD</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_SMLL</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_DRG/MIND</t>
+  </si>
+  <si>
+    <t>FR_MED/REGLTN</t>
+  </si>
+  <si>
+    <t>GEN/SUPRTN</t>
+  </si>
+  <si>
+    <t>REC/PRVCNP</t>
+  </si>
+  <si>
+    <t>RSC/MEDEVC</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_CNT</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_MED</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PARAMD</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PPL/GRP</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PSYPHY</t>
+  </si>
+  <si>
+    <t>INT/RECCE</t>
+  </si>
+  <si>
+    <t>SAV</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_TRNSP/AMB</t>
+  </si>
+  <si>
+    <t>GEN/TRNSP</t>
+  </si>
+  <si>
+    <t>GEN/TRNSP/FR_SECNDRY</t>
+  </si>
+  <si>
+    <t>GEN/TRNSPN</t>
+  </si>
+  <si>
+    <t>OPR/LOG</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PPL/OBS</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_CLRACCSS</t>
   </si>
 </sst>
 </file>
@@ -931,6 +931,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1260,7 +1264,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1304,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -1329,7 +1333,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -1359,23 +1363,23 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="11"/>
@@ -1383,49 +1387,49 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1433,62 +1437,62 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1496,10 +1500,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1507,10 +1511,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1518,10 +1522,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1529,10 +1533,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1540,10 +1544,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1551,10 +1555,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1562,49 +1566,49 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1612,10 +1616,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1623,10 +1627,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1634,62 +1638,62 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="7" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="7"/>
@@ -1697,10 +1701,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1708,36 +1712,36 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1745,79 +1749,79 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="E47" s="7"/>
     </row>
@@ -2001,67 +2005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2475,33 +2418,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FED4B9AA-8877-43C0-9BF1-4CF4C039AF65}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2519,4 +2497,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.02.16 10:59] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="473" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C50C4EBB-4983-4C0A-A415-EA981A5A3BF2}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AFE3A7F-315D-4231-8E6C-F60EF03377C4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
@@ -390,13 +390,7 @@
     <t>SAV</t>
   </si>
   <si>
-    <t>FSTT/TA/FR_TRNSP/AMB</t>
-  </si>
-  <si>
-    <t>GEN/TRNSP</t>
-  </si>
-  <si>
-    <t>GEN/TRNSP/FR_SECNDRY</t>
+    <t>GEN/TRNSPN</t>
   </si>
   <si>
     <t>OPR/LOG</t>
@@ -1760,6 +1754,12 @@
   <si>
     <t xml:space="preserve">Lorsque le SAMU fait une demande de concours vers un autre partenaire en utilisant ce type, cela doit être interprétée comme une demande de transport d'une personne. 
 Lorsqu'un partenaire (ex. SIS) fait une demande de concours vers le SAMU en utilisant ce type, cela doit être interprétée comme une demande de transport médicalisé d'une personne. </t>
+  </si>
+  <si>
+    <t>GEN/TRNSPN/FR_SECNDRY</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_TRNSPN/AMB</t>
   </si>
 </sst>
 </file>
@@ -2690,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,7 +2759,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -2799,7 +2799,7 @@
         <v>61</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>117</v>
+        <v>573</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>56</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="40" spans="1:5" s="14" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>57</v>
@@ -3165,12 +3165,12 @@
         <v>77</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>119</v>
+        <v>572</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>58</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>59</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>60</v>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>84</v>
@@ -3222,766 +3222,766 @@
     </row>
     <row r="45" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>123</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>128</v>
       </c>
       <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>131</v>
       </c>
       <c r="E47" s="27"/>
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>132</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>134</v>
       </c>
       <c r="E48" s="27"/>
     </row>
     <row r="49" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>137</v>
       </c>
       <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="E50" s="27"/>
     </row>
     <row r="51" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>143</v>
       </c>
       <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>149</v>
       </c>
       <c r="E53" s="27"/>
     </row>
     <row r="54" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>155</v>
       </c>
       <c r="E55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="E56" s="27"/>
     </row>
     <row r="57" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="E57" s="27"/>
     </row>
     <row r="58" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>164</v>
       </c>
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>167</v>
       </c>
       <c r="E59" s="27"/>
     </row>
     <row r="60" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="17" t="s">
         <v>168</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>170</v>
       </c>
       <c r="E60" s="27"/>
     </row>
     <row r="61" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>173</v>
       </c>
       <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>177</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>179</v>
       </c>
       <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D64" s="17" t="s">
         <v>180</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>182</v>
       </c>
       <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>185</v>
       </c>
       <c r="E65" s="27"/>
     </row>
     <row r="66" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>188</v>
       </c>
       <c r="E66" s="27"/>
     </row>
     <row r="67" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="E67" s="27"/>
     </row>
     <row r="68" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" s="17" t="s">
         <v>192</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>194</v>
       </c>
       <c r="E68" s="27"/>
     </row>
     <row r="69" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" s="17" t="s">
         <v>195</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>197</v>
       </c>
       <c r="E69" s="27"/>
     </row>
     <row r="70" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="E70" s="27"/>
     </row>
     <row r="71" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D71" s="17" t="s">
         <v>201</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>203</v>
       </c>
       <c r="E71" s="27"/>
     </row>
     <row r="72" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D72" s="17" t="s">
         <v>204</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>206</v>
       </c>
       <c r="E72" s="27"/>
     </row>
     <row r="73" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" s="17" t="s">
         <v>207</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>209</v>
       </c>
       <c r="E73" s="27"/>
     </row>
     <row r="74" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74" s="17" t="s">
         <v>210</v>
-      </c>
-      <c r="B74" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="E74" s="27"/>
     </row>
     <row r="75" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D75" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="B75" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>215</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D76" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="E76" s="27"/>
     </row>
     <row r="77" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D77" s="17" t="s">
         <v>219</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>221</v>
       </c>
       <c r="E77" s="27"/>
     </row>
     <row r="78" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D78" s="17" t="s">
         <v>222</v>
-      </c>
-      <c r="B78" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>224</v>
       </c>
       <c r="E78" s="27"/>
     </row>
     <row r="79" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D79" s="17" t="s">
         <v>225</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>227</v>
       </c>
       <c r="E79" s="27"/>
     </row>
     <row r="80" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" s="17" t="s">
         <v>228</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>230</v>
       </c>
       <c r="E80" s="27"/>
     </row>
     <row r="81" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D81" s="17" t="s">
         <v>231</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>233</v>
       </c>
       <c r="E81" s="27"/>
     </row>
     <row r="82" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="D82" s="17" t="s">
         <v>234</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="E82" s="27"/>
     </row>
     <row r="83" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="17" t="s">
         <v>237</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>239</v>
       </c>
       <c r="E83" s="27"/>
     </row>
     <row r="84" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D84" s="17" t="s">
         <v>240</v>
-      </c>
-      <c r="B84" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>242</v>
       </c>
       <c r="E84" s="27"/>
     </row>
     <row r="85" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D85" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>245</v>
       </c>
       <c r="E85" s="27"/>
     </row>
     <row r="86" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D86" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>248</v>
       </c>
       <c r="E86" s="27"/>
     </row>
     <row r="87" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="D87" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D87" s="17" t="s">
-        <v>251</v>
       </c>
       <c r="E87" s="27"/>
     </row>
     <row r="88" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D88" s="17" t="s">
         <v>252</v>
-      </c>
-      <c r="B88" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>254</v>
       </c>
       <c r="E88" s="27"/>
     </row>
     <row r="89" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D89" s="17" t="s">
         <v>255</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>257</v>
       </c>
       <c r="E89" s="27"/>
     </row>
     <row r="90" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="D90" s="17" t="s">
         <v>258</v>
-      </c>
-      <c r="B90" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>260</v>
       </c>
       <c r="E90" s="27"/>
     </row>
     <row r="91" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="D91" s="17" t="s">
         <v>261</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D91" s="17" t="s">
-        <v>263</v>
       </c>
       <c r="E91" s="27"/>
     </row>
     <row r="92" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="D92" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="B92" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="D92" s="17" t="s">
-        <v>266</v>
       </c>
       <c r="E92" s="27"/>
     </row>
     <row r="93" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D93" s="17" t="s">
         <v>267</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="D93" s="17" t="s">
-        <v>269</v>
       </c>
       <c r="E93" s="27"/>
     </row>
     <row r="94" spans="1:5" s="14" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="D94" s="17" t="s">
-        <v>272</v>
       </c>
       <c r="E94" s="27"/>
     </row>
     <row r="95" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D95" s="17" t="s">
         <v>273</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="D95" s="17" t="s">
-        <v>275</v>
       </c>
       <c r="E95" s="27"/>
     </row>
@@ -3990,1507 +3990,1507 @@
         <v>87</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E96" s="27"/>
     </row>
     <row r="97" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="D97" s="17" t="s">
         <v>278</v>
-      </c>
-      <c r="B97" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="D97" s="17" t="s">
-        <v>280</v>
       </c>
       <c r="E97" s="27"/>
     </row>
     <row r="98" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D98" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="B98" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="D98" s="17" t="s">
-        <v>283</v>
       </c>
       <c r="E98" s="27"/>
     </row>
     <row r="99" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" s="17" t="s">
         <v>284</v>
-      </c>
-      <c r="B99" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="D99" s="17" t="s">
-        <v>286</v>
       </c>
       <c r="E99" s="27"/>
     </row>
     <row r="100" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="D100" s="17" t="s">
-        <v>289</v>
       </c>
       <c r="E100" s="27"/>
     </row>
     <row r="101" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C101" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="D101" s="17" t="s">
         <v>290</v>
-      </c>
-      <c r="B101" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="D101" s="17" t="s">
-        <v>292</v>
       </c>
       <c r="E101" s="27"/>
     </row>
     <row r="102" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="D102" s="17" t="s">
         <v>293</v>
-      </c>
-      <c r="B102" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="D102" s="17" t="s">
-        <v>295</v>
       </c>
       <c r="E102" s="27"/>
     </row>
     <row r="103" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D103" s="17" t="s">
         <v>296</v>
-      </c>
-      <c r="B103" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="D103" s="17" t="s">
-        <v>298</v>
       </c>
       <c r="E103" s="27"/>
     </row>
     <row r="104" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="D104" s="17" t="s">
         <v>299</v>
-      </c>
-      <c r="B104" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="D104" s="17" t="s">
-        <v>301</v>
       </c>
       <c r="E104" s="27"/>
     </row>
     <row r="105" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="D105" s="17" t="s">
         <v>302</v>
-      </c>
-      <c r="B105" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="D105" s="17" t="s">
-        <v>304</v>
       </c>
       <c r="E105" s="27"/>
     </row>
     <row r="106" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="D106" s="17" t="s">
         <v>305</v>
-      </c>
-      <c r="B106" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="D106" s="17" t="s">
-        <v>307</v>
       </c>
       <c r="E106" s="27"/>
     </row>
     <row r="107" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="D107" s="17" t="s">
         <v>308</v>
-      </c>
-      <c r="B107" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="D107" s="17" t="s">
-        <v>310</v>
       </c>
       <c r="E107" s="27"/>
     </row>
     <row r="108" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="D108" s="17" t="s">
         <v>311</v>
-      </c>
-      <c r="B108" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="D108" s="17" t="s">
-        <v>313</v>
       </c>
       <c r="E108" s="27"/>
     </row>
     <row r="109" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D109" s="17" t="s">
         <v>314</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="D109" s="17" t="s">
-        <v>316</v>
       </c>
       <c r="E109" s="27"/>
     </row>
     <row r="110" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D110" s="17" t="s">
         <v>317</v>
-      </c>
-      <c r="B110" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="D110" s="17" t="s">
-        <v>319</v>
       </c>
       <c r="E110" s="27"/>
     </row>
     <row r="111" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D111" s="17" t="s">
         <v>320</v>
-      </c>
-      <c r="B111" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="D111" s="17" t="s">
-        <v>322</v>
       </c>
       <c r="E111" s="27"/>
     </row>
     <row r="112" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="D112" s="17" t="s">
         <v>323</v>
-      </c>
-      <c r="B112" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="D112" s="17" t="s">
-        <v>325</v>
       </c>
       <c r="E112" s="27"/>
     </row>
     <row r="113" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="D113" s="17" t="s">
         <v>326</v>
-      </c>
-      <c r="B113" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="D113" s="17" t="s">
-        <v>328</v>
       </c>
       <c r="E113" s="27"/>
     </row>
     <row r="114" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="D114" s="17" t="s">
         <v>329</v>
-      </c>
-      <c r="B114" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="D114" s="17" t="s">
-        <v>331</v>
       </c>
       <c r="E114" s="27"/>
     </row>
     <row r="115" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="D115" s="17" t="s">
         <v>332</v>
-      </c>
-      <c r="B115" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="D115" s="17" t="s">
-        <v>334</v>
       </c>
       <c r="E115" s="27"/>
     </row>
     <row r="116" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="D116" s="17" t="s">
         <v>335</v>
-      </c>
-      <c r="B116" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="D116" s="17" t="s">
-        <v>337</v>
       </c>
       <c r="E116" s="27"/>
     </row>
     <row r="117" spans="1:5" s="14" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="D117" s="17" t="s">
         <v>338</v>
-      </c>
-      <c r="B117" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="D117" s="17" t="s">
-        <v>340</v>
       </c>
       <c r="E117" s="27"/>
     </row>
     <row r="118" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D118" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="B118" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="D118" s="17" t="s">
-        <v>343</v>
       </c>
       <c r="E118" s="27"/>
     </row>
     <row r="119" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="D119" s="17" t="s">
         <v>344</v>
-      </c>
-      <c r="B119" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="D119" s="17" t="s">
-        <v>346</v>
       </c>
       <c r="E119" s="27"/>
     </row>
     <row r="120" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C120" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D120" s="17" t="s">
         <v>347</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="D120" s="17" t="s">
-        <v>349</v>
       </c>
       <c r="E120" s="27"/>
     </row>
     <row r="121" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C121" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D121" s="17" t="s">
         <v>350</v>
-      </c>
-      <c r="B121" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="D121" s="17" t="s">
-        <v>352</v>
       </c>
       <c r="E121" s="27"/>
     </row>
     <row r="122" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D122" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E122" s="27"/>
     </row>
     <row r="123" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C123" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="D123" s="17" t="s">
         <v>355</v>
-      </c>
-      <c r="B123" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="D123" s="17" t="s">
-        <v>357</v>
       </c>
       <c r="E123" s="27"/>
     </row>
     <row r="124" spans="1:5" s="14" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="D124" s="17" t="s">
         <v>358</v>
-      </c>
-      <c r="B124" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C124" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="D124" s="17" t="s">
-        <v>360</v>
       </c>
       <c r="E124" s="27"/>
     </row>
     <row r="125" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="D125" s="17" t="s">
         <v>361</v>
-      </c>
-      <c r="B125" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C125" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="D125" s="17" t="s">
-        <v>363</v>
       </c>
       <c r="E125" s="27"/>
     </row>
     <row r="126" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C126" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="D126" s="17" t="s">
         <v>364</v>
-      </c>
-      <c r="B126" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C126" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="D126" s="17" t="s">
-        <v>366</v>
       </c>
       <c r="E126" s="27"/>
     </row>
     <row r="127" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="D127" s="17" t="s">
         <v>367</v>
-      </c>
-      <c r="B127" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C127" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="D127" s="17" t="s">
-        <v>369</v>
       </c>
       <c r="E127" s="27"/>
     </row>
     <row r="128" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="D128" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="B128" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C128" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="D128" s="17" t="s">
-        <v>372</v>
       </c>
       <c r="E128" s="27"/>
     </row>
     <row r="129" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C129" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D129" s="17" t="s">
         <v>373</v>
-      </c>
-      <c r="B129" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C129" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="D129" s="17" t="s">
-        <v>375</v>
       </c>
       <c r="E129" s="27"/>
     </row>
     <row r="130" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C130" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="D130" s="17" t="s">
         <v>376</v>
-      </c>
-      <c r="B130" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="D130" s="17" t="s">
-        <v>378</v>
       </c>
       <c r="E130" s="27"/>
     </row>
     <row r="131" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D131" s="17" t="s">
         <v>379</v>
-      </c>
-      <c r="B131" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C131" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="D131" s="17" t="s">
-        <v>381</v>
       </c>
       <c r="E131" s="27"/>
     </row>
     <row r="132" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="D132" s="17" t="s">
         <v>382</v>
-      </c>
-      <c r="B132" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="D132" s="17" t="s">
-        <v>384</v>
       </c>
       <c r="E132" s="27"/>
     </row>
     <row r="133" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C133" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D133" s="17" t="s">
         <v>385</v>
-      </c>
-      <c r="B133" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C133" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="D133" s="17" t="s">
-        <v>387</v>
       </c>
       <c r="E133" s="27"/>
     </row>
     <row r="134" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="D134" s="17" t="s">
         <v>388</v>
-      </c>
-      <c r="B134" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C134" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="D134" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="E134" s="27"/>
     </row>
     <row r="135" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="D135" s="17" t="s">
         <v>391</v>
-      </c>
-      <c r="B135" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C135" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="D135" s="17" t="s">
-        <v>393</v>
       </c>
       <c r="E135" s="27"/>
     </row>
     <row r="136" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="B136" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="D136" s="17" t="s">
         <v>394</v>
-      </c>
-      <c r="B136" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="D136" s="17" t="s">
-        <v>396</v>
       </c>
       <c r="E136" s="27"/>
     </row>
     <row r="137" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D137" s="17"/>
       <c r="E137" s="27"/>
     </row>
     <row r="138" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D138" s="17"/>
       <c r="E138" s="27"/>
     </row>
     <row r="139" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="D139" s="17" t="s">
         <v>401</v>
-      </c>
-      <c r="B139" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="D139" s="17" t="s">
-        <v>403</v>
       </c>
       <c r="E139" s="27"/>
     </row>
     <row r="140" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="D140" s="17" t="s">
         <v>404</v>
-      </c>
-      <c r="B140" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C140" s="15" t="s">
-        <v>405</v>
-      </c>
-      <c r="D140" s="17" t="s">
-        <v>406</v>
       </c>
       <c r="E140" s="27"/>
     </row>
     <row r="141" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="B141" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="D141" s="17" t="s">
         <v>407</v>
-      </c>
-      <c r="B141" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C141" s="15" t="s">
-        <v>408</v>
-      </c>
-      <c r="D141" s="17" t="s">
-        <v>409</v>
       </c>
       <c r="E141" s="27"/>
     </row>
     <row r="142" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D142" s="17" t="s">
         <v>410</v>
-      </c>
-      <c r="B142" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C142" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="D142" s="17" t="s">
-        <v>412</v>
       </c>
       <c r="E142" s="27"/>
     </row>
     <row r="143" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D143" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E143" s="27"/>
     </row>
     <row r="144" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="D144" s="17" t="s">
         <v>415</v>
-      </c>
-      <c r="B144" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C144" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="D144" s="17" t="s">
-        <v>417</v>
       </c>
       <c r="E144" s="27"/>
     </row>
     <row r="145" spans="1:5" s="14" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="D145" s="17" t="s">
         <v>418</v>
-      </c>
-      <c r="B145" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C145" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="D145" s="17" t="s">
-        <v>420</v>
       </c>
       <c r="E145" s="27"/>
     </row>
     <row r="146" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="D146" s="17" t="s">
         <v>421</v>
-      </c>
-      <c r="B146" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C146" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="D146" s="17" t="s">
-        <v>423</v>
       </c>
       <c r="E146" s="27"/>
     </row>
     <row r="147" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="D147" s="17" t="s">
         <v>424</v>
-      </c>
-      <c r="B147" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C147" s="15" t="s">
-        <v>425</v>
-      </c>
-      <c r="D147" s="17" t="s">
-        <v>426</v>
       </c>
       <c r="E147" s="27"/>
     </row>
     <row r="148" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="D148" s="17" t="s">
         <v>427</v>
-      </c>
-      <c r="B148" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="D148" s="17" t="s">
-        <v>429</v>
       </c>
       <c r="E148" s="27"/>
     </row>
     <row r="149" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="D149" s="17" t="s">
         <v>430</v>
-      </c>
-      <c r="B149" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>431</v>
-      </c>
-      <c r="D149" s="17" t="s">
-        <v>432</v>
       </c>
       <c r="E149" s="27"/>
     </row>
     <row r="150" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="B150" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="D150" s="17" t="s">
         <v>433</v>
-      </c>
-      <c r="B150" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C150" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="D150" s="17" t="s">
-        <v>435</v>
       </c>
       <c r="E150" s="27"/>
     </row>
     <row r="151" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="B151" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C151" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="D151" s="17" t="s">
         <v>436</v>
-      </c>
-      <c r="B151" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C151" s="15" t="s">
-        <v>437</v>
-      </c>
-      <c r="D151" s="17" t="s">
-        <v>438</v>
       </c>
       <c r="E151" s="27"/>
     </row>
     <row r="152" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A152" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="B152" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C152" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="D152" s="17" t="s">
         <v>439</v>
-      </c>
-      <c r="B152" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C152" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="D152" s="17" t="s">
-        <v>441</v>
       </c>
       <c r="E152" s="27"/>
     </row>
     <row r="153" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A153" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B153" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="D153" s="17" t="s">
         <v>442</v>
-      </c>
-      <c r="B153" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C153" s="15" t="s">
-        <v>443</v>
-      </c>
-      <c r="D153" s="17" t="s">
-        <v>444</v>
       </c>
       <c r="E153" s="27"/>
     </row>
     <row r="154" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="D154" s="17" t="s">
         <v>445</v>
-      </c>
-      <c r="B154" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C154" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="D154" s="17" t="s">
-        <v>447</v>
       </c>
       <c r="E154" s="27"/>
     </row>
     <row r="155" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A155" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C155" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="D155" s="17" t="s">
         <v>448</v>
-      </c>
-      <c r="B155" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C155" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="D155" s="17" t="s">
-        <v>450</v>
       </c>
       <c r="E155" s="27"/>
     </row>
     <row r="156" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="B156" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="D156" s="17" t="s">
         <v>451</v>
-      </c>
-      <c r="B156" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C156" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="D156" s="17" t="s">
-        <v>453</v>
       </c>
       <c r="E156" s="27"/>
     </row>
     <row r="157" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A157" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="B157" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C157" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="D157" s="17" t="s">
         <v>454</v>
-      </c>
-      <c r="B157" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C157" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="D157" s="17" t="s">
-        <v>456</v>
       </c>
       <c r="E157" s="27"/>
     </row>
     <row r="158" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A158" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C158" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="D158" s="17" t="s">
         <v>457</v>
-      </c>
-      <c r="B158" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C158" s="15" t="s">
-        <v>458</v>
-      </c>
-      <c r="D158" s="17" t="s">
-        <v>459</v>
       </c>
       <c r="E158" s="27"/>
     </row>
     <row r="159" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C159" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="D159" s="17" t="s">
         <v>460</v>
-      </c>
-      <c r="B159" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C159" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="D159" s="17" t="s">
-        <v>462</v>
       </c>
       <c r="E159" s="27"/>
     </row>
     <row r="160" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="B160" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C160" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="D160" s="17" t="s">
         <v>463</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C160" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="D160" s="17" t="s">
-        <v>465</v>
       </c>
       <c r="E160" s="27"/>
     </row>
     <row r="161" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B161" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C161" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D161" s="17" t="s">
         <v>466</v>
-      </c>
-      <c r="B161" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C161" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="D161" s="17" t="s">
-        <v>468</v>
       </c>
       <c r="E161" s="27"/>
     </row>
     <row r="162" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="B162" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C162" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="D162" s="17" t="s">
         <v>469</v>
-      </c>
-      <c r="B162" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C162" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="D162" s="17" t="s">
-        <v>471</v>
       </c>
       <c r="E162" s="27"/>
     </row>
     <row r="163" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="B163" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="D163" s="17" t="s">
         <v>472</v>
-      </c>
-      <c r="B163" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="D163" s="17" t="s">
-        <v>474</v>
       </c>
       <c r="E163" s="27"/>
     </row>
     <row r="164" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="15" t="s">
+        <v>473</v>
+      </c>
+      <c r="B164" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C164" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="D164" s="17" t="s">
         <v>475</v>
-      </c>
-      <c r="B164" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C164" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="D164" s="17" t="s">
-        <v>477</v>
       </c>
       <c r="E164" s="27"/>
     </row>
     <row r="165" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A165" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="B165" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C165" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="D165" s="17" t="s">
         <v>478</v>
-      </c>
-      <c r="B165" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C165" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="D165" s="17" t="s">
-        <v>480</v>
       </c>
       <c r="E165" s="27"/>
     </row>
     <row r="166" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="B166" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C166" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D166" s="17" t="s">
         <v>481</v>
-      </c>
-      <c r="B166" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C166" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="D166" s="17" t="s">
-        <v>483</v>
       </c>
       <c r="E166" s="27"/>
     </row>
     <row r="167" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A167" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="B167" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C167" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="D167" s="17" t="s">
         <v>484</v>
-      </c>
-      <c r="B167" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C167" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="D167" s="17" t="s">
-        <v>486</v>
       </c>
       <c r="E167" s="27"/>
     </row>
     <row r="168" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="B168" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C168" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="D168" s="17" t="s">
         <v>487</v>
-      </c>
-      <c r="B168" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C168" s="15" t="s">
-        <v>488</v>
-      </c>
-      <c r="D168" s="17" t="s">
-        <v>489</v>
       </c>
       <c r="E168" s="27"/>
     </row>
     <row r="169" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="B169" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C169" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="D169" s="17" t="s">
         <v>490</v>
-      </c>
-      <c r="B169" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C169" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="D169" s="17" t="s">
-        <v>492</v>
       </c>
       <c r="E169" s="27"/>
     </row>
     <row r="170" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A170" s="15" t="s">
+        <v>491</v>
+      </c>
+      <c r="B170" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C170" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="D170" s="17" t="s">
         <v>493</v>
-      </c>
-      <c r="B170" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C170" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="D170" s="17" t="s">
-        <v>495</v>
       </c>
       <c r="E170" s="27"/>
     </row>
     <row r="171" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B171" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C171" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="D171" s="17" t="s">
         <v>496</v>
-      </c>
-      <c r="B171" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C171" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="D171" s="17" t="s">
-        <v>498</v>
       </c>
       <c r="E171" s="27"/>
     </row>
     <row r="172" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="B172" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C172" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="D172" s="17" t="s">
         <v>499</v>
-      </c>
-      <c r="B172" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C172" s="15" t="s">
-        <v>500</v>
-      </c>
-      <c r="D172" s="17" t="s">
-        <v>501</v>
       </c>
       <c r="E172" s="27"/>
     </row>
     <row r="173" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="B173" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C173" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="D173" s="17" t="s">
         <v>502</v>
-      </c>
-      <c r="B173" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C173" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="D173" s="17" t="s">
-        <v>504</v>
       </c>
       <c r="E173" s="27"/>
     </row>
     <row r="174" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="B174" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C174" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="D174" s="17" t="s">
         <v>505</v>
-      </c>
-      <c r="B174" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C174" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="D174" s="17" t="s">
-        <v>507</v>
       </c>
       <c r="E174" s="27"/>
     </row>
     <row r="175" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="B175" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C175" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="D175" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="B175" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C175" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="D175" s="17" t="s">
-        <v>510</v>
       </c>
       <c r="E175" s="27"/>
     </row>
     <row r="176" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C176" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="D176" s="17" t="s">
         <v>511</v>
-      </c>
-      <c r="B176" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C176" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="D176" s="17" t="s">
-        <v>513</v>
       </c>
       <c r="E176" s="27"/>
     </row>
     <row r="177" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="B177" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C177" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="D177" s="17" t="s">
         <v>514</v>
-      </c>
-      <c r="B177" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C177" s="15" t="s">
-        <v>515</v>
-      </c>
-      <c r="D177" s="17" t="s">
-        <v>516</v>
       </c>
       <c r="E177" s="27"/>
     </row>
     <row r="178" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A178" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B178" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C178" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="D178" s="17" t="s">
         <v>517</v>
-      </c>
-      <c r="B178" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>518</v>
-      </c>
-      <c r="D178" s="17" t="s">
-        <v>519</v>
       </c>
       <c r="E178" s="27"/>
     </row>
     <row r="179" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="B179" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C179" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="D179" s="17" t="s">
         <v>520</v>
-      </c>
-      <c r="B179" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C179" s="15" t="s">
-        <v>521</v>
-      </c>
-      <c r="D179" s="17" t="s">
-        <v>522</v>
       </c>
       <c r="E179" s="27"/>
     </row>
     <row r="180" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="B180" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C180" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D180" s="17" t="s">
         <v>523</v>
-      </c>
-      <c r="B180" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C180" s="15" t="s">
-        <v>524</v>
-      </c>
-      <c r="D180" s="17" t="s">
-        <v>525</v>
       </c>
       <c r="E180" s="27"/>
     </row>
     <row r="181" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="15" t="s">
+        <v>524</v>
+      </c>
+      <c r="B181" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C181" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="D181" s="17" t="s">
         <v>526</v>
-      </c>
-      <c r="B181" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C181" s="15" t="s">
-        <v>527</v>
-      </c>
-      <c r="D181" s="17" t="s">
-        <v>528</v>
       </c>
       <c r="E181" s="27"/>
     </row>
     <row r="182" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D182" s="17"/>
       <c r="E182" s="27"/>
     </row>
     <row r="183" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A183" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="B183" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C183" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="D183" s="17" t="s">
         <v>531</v>
-      </c>
-      <c r="B183" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C183" s="15" t="s">
-        <v>532</v>
-      </c>
-      <c r="D183" s="17" t="s">
-        <v>533</v>
       </c>
       <c r="E183" s="27"/>
     </row>
     <row r="184" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A184" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="B184" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C184" s="15" t="s">
+        <v>533</v>
+      </c>
+      <c r="D184" s="17" t="s">
         <v>534</v>
-      </c>
-      <c r="B184" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C184" s="15" t="s">
-        <v>535</v>
-      </c>
-      <c r="D184" s="17" t="s">
-        <v>536</v>
       </c>
       <c r="E184" s="27"/>
     </row>
     <row r="185" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A185" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="B185" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C185" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="D185" s="17" t="s">
         <v>537</v>
-      </c>
-      <c r="B185" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C185" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="D185" s="17" t="s">
-        <v>539</v>
       </c>
       <c r="E185" s="27"/>
     </row>
     <row r="186" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A186" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="B186" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C186" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="D186" s="17" t="s">
         <v>540</v>
-      </c>
-      <c r="B186" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C186" s="15" t="s">
-        <v>541</v>
-      </c>
-      <c r="D186" s="17" t="s">
-        <v>542</v>
       </c>
       <c r="E186" s="27"/>
     </row>
     <row r="187" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C187" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="D187" s="17" t="s">
         <v>543</v>
-      </c>
-      <c r="B187" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C187" s="15" t="s">
-        <v>544</v>
-      </c>
-      <c r="D187" s="17" t="s">
-        <v>545</v>
       </c>
       <c r="E187" s="27"/>
     </row>
     <row r="188" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A188" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C188" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="D188" s="17" t="s">
         <v>546</v>
-      </c>
-      <c r="B188" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C188" s="15" t="s">
-        <v>547</v>
-      </c>
-      <c r="D188" s="17" t="s">
-        <v>548</v>
       </c>
       <c r="E188" s="27"/>
     </row>
     <row r="189" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A189" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="B189" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C189" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D189" s="17" t="s">
         <v>549</v>
-      </c>
-      <c r="B189" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C189" s="15" t="s">
-        <v>550</v>
-      </c>
-      <c r="D189" s="17" t="s">
-        <v>551</v>
       </c>
       <c r="E189" s="27"/>
     </row>
     <row r="190" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A190" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="B190" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C190" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="D190" s="17" t="s">
         <v>552</v>
-      </c>
-      <c r="B190" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C190" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="D190" s="17" t="s">
-        <v>554</v>
       </c>
       <c r="E190" s="27"/>
     </row>
     <row r="191" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A191" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B191" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C191" s="15" t="s">
+        <v>554</v>
+      </c>
+      <c r="D191" s="17" t="s">
         <v>555</v>
-      </c>
-      <c r="B191" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C191" s="15" t="s">
-        <v>556</v>
-      </c>
-      <c r="D191" s="17" t="s">
-        <v>557</v>
       </c>
       <c r="E191" s="27"/>
     </row>
     <row r="192" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A192" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="B192" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C192" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="D192" s="17" t="s">
         <v>558</v>
-      </c>
-      <c r="B192" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C192" s="15" t="s">
-        <v>559</v>
-      </c>
-      <c r="D192" s="17" t="s">
-        <v>560</v>
       </c>
       <c r="E192" s="27"/>
     </row>
     <row r="193" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A193" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="B193" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C193" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="D193" s="17" t="s">
         <v>561</v>
-      </c>
-      <c r="B193" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="C193" s="15" t="s">
-        <v>562</v>
-      </c>
-      <c r="D193" s="17" t="s">
-        <v>563</v>
       </c>
       <c r="E193" s="27"/>
     </row>
     <row r="194" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A194" s="15" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B194" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D194" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E194" s="27"/>
     </row>
     <row r="195" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A195" s="15" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B195" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D195" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E195" s="27"/>
     </row>
     <row r="196" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A196" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="B196" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C196" s="31" t="s">
+        <v>567</v>
+      </c>
+      <c r="D196" s="33" t="s">
         <v>568</v>
-      </c>
-      <c r="B196" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="C196" s="31" t="s">
-        <v>569</v>
-      </c>
-      <c r="D196" s="33" t="s">
-        <v>570</v>
       </c>
       <c r="E196" s="34"/>
     </row>

</xml_diff>

<commit_message>
[24.07.29 18:44] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -5674,8 +5674,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5a233c5be867259e7f523794110a7773">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71fc54e2a62b1985aea6da9d2195ce0c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -5738,12 +5738,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -5856,7 +5856,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -5875,7 +5875,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -5948,7 +5948,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -5997,8 +5997,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -6149,23 +6149,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FED4B9AA-8877-43C0-9BF1-4CF4C039AF65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E667A7-F4F8-4400-8D2D-A6FF373AD471}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.07.30 19:12] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9A7AD4-C0C3-4288-8035-3CDDBE7CCD26}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{996BAC3A-153D-4895-A843-57E02C19F9A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">Lorsque ce type est sélectionné, le champ MISSION.PRIORITY doit être complété pour que le partenaire distingue la prise en charge secouriste non urgente (priorité = 1) de la prise en charge secouriste urgente (priorité = 5). </t>
   </si>
   <si>
-    <t>/SAV/ASC</t>
-  </si>
-  <si>
     <t>BESOIN SECOURISTE / PERSONNE(S) BLESSE(ES)</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>S'agit d'une demande d'engagement de ressources en vue de prendre en charge un patient/victime par des secouristes</t>
   </si>
   <si>
-    <t>/FR_MED/REGLTN</t>
-  </si>
-  <si>
     <t>REGULATION MEDICALE</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>S'agit d'une demande de solicitation du SAMU en vue s'assurer une régulation médicale pour engager ou non des ressources</t>
   </si>
   <si>
-    <t>/GEN/SUPRTN</t>
-  </si>
-  <si>
     <t>SOUTIEN MEDICO PSYCHOLOGIQUE</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
     <t>S'agit d'une demande d'engagement de ressources en vue d'apporter à un patient/victime un soutien médico psychologique</t>
   </si>
   <si>
-    <t>/SAV/AR/FR_MED</t>
-  </si>
-  <si>
     <t>MEDICALISATION OU EVALUATION MEDICALE</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>S'agit d'une demande d'engagement de ressources en vue de prendre en charge un patient/victime par une équipe médicale</t>
   </si>
   <si>
-    <t>/SAV/AR/FR_PARAMD</t>
-  </si>
-  <si>
     <t>PARA MEDICALISATION</t>
   </si>
   <si>
@@ -204,18 +189,12 @@
     <t>S'agit d'une demande d'engagement de ressources en vue de prendre en charge un patient/victime par une équipe para médicale</t>
   </si>
   <si>
-    <t>/SAV</t>
-  </si>
-  <si>
     <t>AUTRE</t>
   </si>
   <si>
     <t>S'agit d'une demande au SAMU, autre que celles déjà existants (ex. prise en charge d'un problème médico social)</t>
   </si>
   <si>
-    <t>/GEN/TRNSPN</t>
-  </si>
-  <si>
     <t>TRANSPORT DE PERSONNE</t>
   </si>
   <si>
@@ -225,9 +204,6 @@
     <t xml:space="preserve">S'agit du transport d'un patient/victime vers un établissement de santé (ES) à l'aide d'un moyen adapté. </t>
   </si>
   <si>
-    <t>/SAV/SARCSL</t>
-  </si>
-  <si>
     <t>VICTIME ENSEVELIE</t>
   </si>
   <si>
@@ -237,9 +213,6 @@
     <t>Patient/Victime piégé sous des matériaux/matières dont l'abord est rendu difficile (ex. avalanche, silo à grain, fontis, structure, etc.)</t>
   </si>
   <si>
-    <t>/SAV/ASC/FR_PPL/LIFT</t>
-  </si>
-  <si>
     <t>RELEVAGE</t>
   </si>
   <si>
@@ -249,9 +222,6 @@
     <t>Patient/victime au sol dans l'incapacité de se relever par elle-même ou l'aide de ses proches.</t>
   </si>
   <si>
-    <t>/GEN/RECVRY</t>
-  </si>
-  <si>
     <t>DEGAGEMENT DE PERSONNE</t>
   </si>
   <si>
@@ -261,75 +231,48 @@
     <t>Patient/victime bloqué à libérer (ex. désincarcération, personne dans un ascenseur, etc.).</t>
   </si>
   <si>
-    <t>/SAV/RHD</t>
-  </si>
-  <si>
     <t xml:space="preserve">EVACUATION </t>
   </si>
   <si>
     <t>Demander un appui pour évacuation</t>
   </si>
   <si>
-    <t>/FFST/FR_FIRE</t>
-  </si>
-  <si>
     <t>LUTTE INCENDIE</t>
   </si>
   <si>
-    <t>/FSTT/RRHAZ/FR_CO</t>
-  </si>
-  <si>
     <t>MONOXYDE CARBONE</t>
   </si>
   <si>
     <t>Demander une levée de doute CO</t>
   </si>
   <si>
-    <t>/CBRN/TSA</t>
-  </si>
-  <si>
     <t>DOUTE NRBC</t>
   </si>
   <si>
     <t>Demander une levée de doute NRBC</t>
   </si>
   <si>
-    <t>/INT/RECCE/FR_SMLL</t>
-  </si>
-  <si>
     <t>ODEUR SUSPECTE</t>
   </si>
   <si>
     <t>Demander une levée de doute d'odeur/fumée suspecte</t>
   </si>
   <si>
-    <t>/FSTT/TA</t>
-  </si>
-  <si>
     <t>APPUI TECHNIQUE</t>
   </si>
   <si>
     <t>Demander un appui technique</t>
   </si>
   <si>
-    <t>/SAV/AR/FR_PPL/GRP</t>
-  </si>
-  <si>
     <t>NOMBREUSES VICTIMES</t>
   </si>
   <si>
     <t>Demander une prise en charge de nombreuses victimes</t>
   </si>
   <si>
-    <t>/INT/RECCE</t>
-  </si>
-  <si>
     <t>Autre demande de concours au SIS</t>
   </si>
   <si>
-    <t>/GEN/TRNSPN/FR_SECNDRY</t>
-  </si>
-  <si>
     <t>TRANFERT INTERETABLISSEMENT</t>
   </si>
   <si>
@@ -339,31 +282,88 @@
     <t xml:space="preserve">S'agit du transport d'un patient/victime d'un établissement de santé vers un autre à l'aide d'un moyen adapté. </t>
   </si>
   <si>
-    <t>/OPR/LOG</t>
-  </si>
-  <si>
     <t>BRANCARDAGE</t>
   </si>
   <si>
     <t xml:space="preserve">Demander une aide au brancardage </t>
   </si>
   <si>
-    <t>/SAV/AR/FR_PPL/OBS</t>
-  </si>
-  <si>
     <t>TRANSPORT BARIATRIQUE</t>
   </si>
   <si>
     <t>Demander un transport bariatrique</t>
   </si>
   <si>
-    <t>/FSTT/TA/FR_CLRACCSS</t>
-  </si>
-  <si>
     <t>OUVERTURE ACCES (DANS LOCAL)</t>
   </si>
   <si>
     <t>Demander l'ouverture d'accès</t>
+  </si>
+  <si>
+    <t>SAV/ASC</t>
+  </si>
+  <si>
+    <t>FR_MED/REGLTN</t>
+  </si>
+  <si>
+    <t>GEN/SUPRTN</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_MED</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PARAMD</t>
+  </si>
+  <si>
+    <t>SAV</t>
+  </si>
+  <si>
+    <t>GEN/TRNSPN</t>
+  </si>
+  <si>
+    <t>SAV/SARCSL</t>
+  </si>
+  <si>
+    <t>SAV/ASC/FR_PPL/LIFT</t>
+  </si>
+  <si>
+    <t>GEN/RECVRY</t>
+  </si>
+  <si>
+    <t>SAV/RHD</t>
+  </si>
+  <si>
+    <t>FFST/FR_FIRE</t>
+  </si>
+  <si>
+    <t>FSTT/RRHAZ/FR_CO</t>
+  </si>
+  <si>
+    <t>CBRN/TSA</t>
+  </si>
+  <si>
+    <t>INT/RECCE/FR_SMLL</t>
+  </si>
+  <si>
+    <t>FSTT/TA</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PPL/GRP</t>
+  </si>
+  <si>
+    <t>INT/RECCE</t>
+  </si>
+  <si>
+    <t>GEN/TRNSPN/FR_SECNDRY</t>
+  </si>
+  <si>
+    <t>OPR/LOG</t>
+  </si>
+  <si>
+    <t>SAV/AR/FR_PPL/OBS</t>
+  </si>
+  <si>
+    <t>FSTT/TA/FR_CLRACCSS</t>
   </si>
 </sst>
 </file>
@@ -532,146 +532,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -856,6 +716,146 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
@@ -906,24 +906,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F75B1DA5-9891-4F6A-AB67-59BFCEA39278}" name="Table134579113" displayName="Table134579113" ref="A9:E31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A9:E31" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D3C2EF9F-0A39-4713-AB81-BA1DFEE125BD}" name="Code" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BDEDD48A-6D09-407F-B330-F11B697A342A}" name="Libellé niveau 1" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9EAEB59C-E528-479D-B4DB-07FD7318AA29}" name="Libellé niveau 2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{79972EBC-A878-42E5-AB0B-CDC61DFBF42E}" name="Description" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{5092645F-AF03-4ECF-B094-0195250A70F4}" name="Commentaire" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{D3C2EF9F-0A39-4713-AB81-BA1DFEE125BD}" name="Code" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{BDEDD48A-6D09-407F-B330-F11B697A342A}" name="Libellé niveau 1" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{9EAEB59C-E528-479D-B4DB-07FD7318AA29}" name="Libellé niveau 2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{79972EBC-A878-42E5-AB0B-CDC61DFBF42E}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5092645F-AF03-4ECF-B094-0195250A70F4}" name="Commentaire" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A9:D15" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{551A8DD3-5DD1-4ECC-B023-12CD9EFCF3B9}" name="Code" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BA9EB287-2815-4894-9C7A-3A1F78EA64E2}" name="Libellé niveau 1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{8983F048-A7D9-4527-8A44-F61CAF1F330A}" name="Description" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{32E442D7-7F8D-432D-BD88-1191DD3FE2FC}" name="Commentaire" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{551A8DD3-5DD1-4ECC-B023-12CD9EFCF3B9}" name="Code" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BA9EB287-2815-4894-9C7A-3A1F78EA64E2}" name="Libellé niveau 1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8983F048-A7D9-4527-8A44-F61CAF1F330A}" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{32E442D7-7F8D-432D-BD88-1191DD3FE2FC}" name="Commentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,16 +1327,16 @@
     </row>
     <row r="10" spans="1:5" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>34</v>
@@ -1344,158 +1344,158 @@
     </row>
     <row r="11" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="D11" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>42</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>46</v>
       </c>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>29</v>
@@ -1505,132 +1505,132 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -1815,58 +1815,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2280,6 +2228,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2290,25 +2290,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1349BA55-BFED-4FC1-8096-AFA7D69A4FE0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1349BA55-BFED-4FC1-8096-AFA7D69A4FE0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.09.13 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI MISSION.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,6 +2229,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -2280,15 +2289,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1349BA55-BFED-4FC1-8096-AFA7D69A4FE0}">
   <ds:schemaRefs>
@@ -2310,27 +2310,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98F885D4-EF3D-4686-B5F6-1FDD2BF41E71}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3BBB1E-C9DF-4117-9187-A8DD65EB643C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>